<commit_message>
created a function, analyzed all genders
</commit_message>
<xml_diff>
--- a/The Impact of Female Role Models on the Retention of Women in Computer Science_March 20, 2024_14.03.xlsx
+++ b/The Impact of Female Role Models on the Retention of Women in Computer Science_March 20, 2024_14.03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/asamsom_uvm_edu/Documents/UVM/2024 Spring/HCOL Thesis/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/asamsom_uvm_edu/Documents/UVM/2024 Spring/HCOL Thesis/Data/honors_thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{7585DF51-3DF5-420E-B59C-6EE8E955B6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="The Impact of Female Role Model" sheetId="1" r:id="rId1"/>
@@ -984,7 +984,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1843,11 +1843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="B190" sqref="B190"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1855,7 +1855,7 @@
     <col min="1" max="1" width="51.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>